<commit_message>
Will be editing code to take acoount or townhouses; Excel sheet of Georgia properties finished with Updates Coming
</commit_message>
<xml_diff>
--- a/South Carolina/SC - RealEstateData.xlsx
+++ b/South Carolina/SC - RealEstateData.xlsx
@@ -3088,12 +3088,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3117,30 +3117,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3153,24 +3131,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3224,13 +3203,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -3238,7 +3210,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3252,9 +3232,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3269,13 +3262,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3287,31 +3286,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3329,13 +3328,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3347,37 +3394,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3395,7 +3424,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3407,49 +3436,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3541,15 +3534,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -3575,61 +3559,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -3638,88 +3631,88 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4076,8 +4069,8 @@
   <sheetPr/>
   <dimension ref="A1:F398"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F1573"/>
+    <sheetView tabSelected="1" topLeftCell="A352" workbookViewId="0">
+      <selection activeCell="A352" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>

</xml_diff>